<commit_message>
Setup modeling of 2016 Super Rugby season
</commit_message>
<xml_diff>
--- a/2015WorldCup/predictions/Round_SF_Matrix.xlsx
+++ b/2015WorldCup/predictions/Round_SF_Matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="4" r:id="rId1"/>
@@ -705,36 +705,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,6 +725,36 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,7 +1062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1170,14 +1170,14 @@
         <f>C9*(C11*E3+C12*F3)</f>
         <v>0.15175204850533869</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="44">
         <f>D9</f>
         <v>0.15175204850533869</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="55">
+      <c r="H9" s="45">
         <v>0.47212594828903082</v>
       </c>
     </row>
@@ -1193,14 +1193,14 @@
         <f>C10*(C11*E4+C12*F4)</f>
         <v>0.47212594828903082</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="44">
         <f t="shared" ref="E10:E12" si="0">D10</f>
         <v>0.47212594828903082</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="55">
+      <c r="H10" s="45">
         <v>0.25824487766417548</v>
       </c>
     </row>
@@ -1216,14 +1216,14 @@
         <f>C11*(C9*C5+C10*D5)</f>
         <v>0.11787712554145501</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="44">
         <f t="shared" si="0"/>
         <v>0.11787712554145501</v>
       </c>
       <c r="G11" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="55">
+      <c r="H11" s="45">
         <v>0.15175204850533869</v>
       </c>
     </row>
@@ -1239,14 +1239,14 @@
         <f>C12*(C9*C6+C10*D6)</f>
         <v>0.25824487766417548</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="44">
         <f t="shared" si="0"/>
         <v>0.25824487766417548</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="55">
+      <c r="H12" s="45">
         <v>0.11787712554145501</v>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -1284,85 +1284,85 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="50"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="48"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="38"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" s="15"/>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="46"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="46"/>
+      <c r="I3" s="47"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
-      <c r="M3" s="47" t="s">
+      <c r="M3" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="46"/>
+      <c r="N3" s="47"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="15"/>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="49"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="49"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="44"/>
+      <c r="N4" s="49"/>
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="15"/>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="42"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="40"/>
+      <c r="I5" s="55"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
-      <c r="M5" s="39" t="s">
+      <c r="M5" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="38"/>
+      <c r="N5" s="51"/>
       <c r="O5" s="37"/>
     </row>
     <row r="6" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1543,32 +1543,32 @@
     </row>
     <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="15"/>
-      <c r="C14" s="52">
+      <c r="C14" s="42">
         <v>23</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="41">
         <v>19</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="F14" s="52">
+      <c r="F14" s="42">
         <v>62</v>
       </c>
-      <c r="G14" s="53">
+      <c r="G14" s="43">
         <v>13</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="53">
+      <c r="J14" s="43">
         <v>20</v>
       </c>
-      <c r="K14" s="52">
+      <c r="K14" s="42">
         <v>43</v>
       </c>
       <c r="L14" s="12"/>
-      <c r="M14" s="52">
+      <c r="M14" s="42">
         <v>35</v>
       </c>
-      <c r="N14" s="51">
+      <c r="N14" s="41">
         <v>34</v>
       </c>
       <c r="O14" s="9"/>

</xml_diff>